<commit_message>
updated PPT2 and Expenses
</commit_message>
<xml_diff>
--- a/Documentation/Expenses.xlsx
+++ b/Documentation/Expenses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Project Manager</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>Facilities/Utilities/Equipments/Furnitures</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>http://us.toshiba.com/</t>
+  </si>
+  <si>
+    <t>https://www.acer.com/ac/en/US/content/home</t>
+  </si>
+  <si>
+    <t>http://weddings.costhelper.com/table-chair-rentals.html</t>
   </si>
 </sst>
 </file>
@@ -206,7 +221,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,11 +246,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -552,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,124 +717,220 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="4">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="10">
-        <v>9000</v>
-      </c>
-      <c r="C15">
-        <v>18</v>
-      </c>
-      <c r="D15" s="10">
-        <f>B15*C15</f>
-        <v>162000</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B16" s="6">
+        <v>9000</v>
+      </c>
+      <c r="C16" s="4">
+        <v>18</v>
+      </c>
+      <c r="D16" s="6">
+        <f>B16*C16</f>
+        <v>162000</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="6">
+        <v>60000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>18</v>
+      </c>
+      <c r="D17" s="6">
+        <f>B17*C17</f>
+        <v>1080000</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="6">
+        <v>30000</v>
+      </c>
+      <c r="C18" s="4">
+        <v>18</v>
+      </c>
+      <c r="D18" s="6">
+        <v>30000</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1500</v>
+      </c>
+      <c r="C19" s="4">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6">
+        <f>B19*C19</f>
+        <v>27000</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="12">
-        <v>2413</v>
-      </c>
-      <c r="C20">
-        <v>18</v>
-      </c>
-      <c r="D20" s="12">
+        <v>23</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1500</v>
+      </c>
+      <c r="C20" s="4">
+        <v>18</v>
+      </c>
+      <c r="D20" s="6">
         <f>B20*C20</f>
-        <v>43434</v>
+        <v>27000</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="12">
-        <v>1797.05</v>
-      </c>
-      <c r="C21">
-        <v>18</v>
-      </c>
-      <c r="D21" s="12">
+        <v>24</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2413</v>
+      </c>
+      <c r="C21" s="4">
+        <v>18</v>
+      </c>
+      <c r="D21" s="6">
         <f>B21*C21</f>
-        <v>32346.899999999998</v>
+        <v>43434</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="12">
-        <v>2568.21</v>
-      </c>
-      <c r="C22">
-        <v>18</v>
-      </c>
-      <c r="D22" s="12">
+        <v>27</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1797.05</v>
+      </c>
+      <c r="C22" s="4">
+        <v>18</v>
+      </c>
+      <c r="D22" s="11">
         <f>B22*C22</f>
-        <v>46227.78</v>
+        <v>32346.899999999998</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2568.21</v>
+      </c>
+      <c r="C23" s="4">
+        <v>18</v>
+      </c>
+      <c r="D23" s="11">
+        <f>B23*C23</f>
+        <v>46227.78</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="13">
+        <f>SUM(D16:D23)</f>
+        <v>1448008.68</v>
       </c>
     </row>
   </sheetData>
@@ -821,12 +939,16 @@
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F5" r:id="rId3"/>
     <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F21" r:id="rId5"/>
-    <hyperlink ref="F15" r:id="rId6"/>
-    <hyperlink ref="F22" r:id="rId7"/>
-    <hyperlink ref="F20" r:id="rId8"/>
+    <hyperlink ref="F22" r:id="rId5"/>
+    <hyperlink ref="F16" r:id="rId6"/>
+    <hyperlink ref="F23" r:id="rId7"/>
+    <hyperlink ref="F21" r:id="rId8"/>
+    <hyperlink ref="F18" r:id="rId9"/>
+    <hyperlink ref="F17" r:id="rId10"/>
+    <hyperlink ref="F19" r:id="rId11"/>
+    <hyperlink ref="F20" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>